<commit_message>
6 reflection and 6 time added
</commit_message>
<xml_diff>
--- a/time/tatyana-malan/6-time.xlsx
+++ b/time/tatyana-malan/6-time.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38">
   <si>
     <t>Sprint 6 Progress Log</t>
   </si>
@@ -91,6 +91,10 @@
   </si>
   <si>
     <t>Break</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#1078 6.0 Minesweeper: and so it begins!
+</t>
   </si>
   <si>
     <t>Sat 16 Dec</t>
@@ -137,12 +141,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,15 +163,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,39 +201,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -225,19 +233,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -250,41 +287,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -296,21 +301,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,19 +346,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.0999786370433668"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -371,170 +536,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="27">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -684,6 +687,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -693,6 +709,32 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -796,6 +838,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -811,59 +888,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -878,12 +902,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -901,134 +943,134 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1062,37 +1104,47 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1411,7 +1463,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1420,9 +1472,10 @@
     <col min="5" max="5" width="16.8571428571429" customWidth="1"/>
     <col min="6" max="6" width="18.5714285714286" customWidth="1"/>
     <col min="7" max="7" width="18.1428571428571" customWidth="1"/>
+    <col min="9" max="9" width="19.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" ht="15.75" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1442,9 +1495,9 @@
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
-      <c r="R1" s="22"/>
+      <c r="R1" s="26"/>
     </row>
-    <row r="2" ht="15.75" spans="1:18">
+    <row r="2" spans="1:18">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
@@ -1463,8 +1516,8 @@
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="24" t="s">
+      <c r="Q2" s="27"/>
+      <c r="R2" s="28" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1515,10 +1568,10 @@
       <c r="P3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="25" t="s">
+      <c r="Q3" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="26"/>
+      <c r="R3" s="30"/>
     </row>
     <row r="4" ht="66" customHeight="1" spans="1:18">
       <c r="A4" s="11" t="s">
@@ -1526,320 +1579,325 @@
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="28"/>
+      <c r="I4" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" ht="51" customHeight="1" spans="1:18">
-      <c r="A5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="15" t="s">
+      <c r="A5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="28"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="32"/>
     </row>
     <row r="6" ht="42" customHeight="1" spans="1:18">
-      <c r="A6" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="15" t="s">
+      <c r="A6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="28"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="32"/>
     </row>
     <row r="7" ht="47" customHeight="1" spans="1:18">
-      <c r="A7" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="15" t="s">
+      <c r="A7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="28"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="32"/>
     </row>
     <row r="8" ht="47" customHeight="1" spans="1:18">
-      <c r="A8" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="15" t="s">
+      <c r="A8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="28"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="32"/>
     </row>
     <row r="9" ht="42" customHeight="1" spans="1:18">
-      <c r="A9" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="15" t="s">
+      <c r="A9" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="28"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="32"/>
     </row>
     <row r="10" ht="45" customHeight="1" spans="1:18">
-      <c r="A10" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="15" t="s">
+      <c r="A10" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="28"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="32"/>
     </row>
     <row r="11" ht="45" customHeight="1" spans="1:18">
-      <c r="A11" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="15" t="s">
+      <c r="A11" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="28"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="32"/>
     </row>
     <row r="12" ht="40" customHeight="1" spans="1:18">
-      <c r="A12" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="15" t="s">
+      <c r="A12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="28"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="32"/>
     </row>
     <row r="13" ht="39" customHeight="1" spans="1:18">
-      <c r="A13" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="15" t="s">
+      <c r="A13" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="28"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="32"/>
     </row>
     <row r="14" ht="44" customHeight="1" spans="1:18">
-      <c r="A14" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="15" t="s">
+      <c r="A14" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="28"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="32"/>
     </row>
     <row r="15" ht="39" customHeight="1" spans="1:18">
-      <c r="A15" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="15" t="s">
+      <c r="A15" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="29"/>
-      <c r="R15" s="28"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="32"/>
     </row>
     <row r="16" ht="45" customHeight="1" spans="1:18">
-      <c r="A16" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="15" t="s">
+      <c r="A16" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="28"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="32"/>
     </row>
     <row r="17" ht="26" customHeight="1" spans="17:18">
       <c r="Q17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R17">
         <v>0</v>

</xml_diff>